<commit_message>
Changed exchange rate for sample country to 100 and currency to LC.
</commit_message>
<xml_diff>
--- a/SourceData/globals/GBModData.xlsx
+++ b/SourceData/globals/GBModData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38224B71-8CDA-4DA5-BC06-35E95BB2FE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1424D40-CB90-4576-BDB0-A23C534A0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryMaster" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3903" uniqueCount="1458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3903" uniqueCount="1459">
   <si>
     <t>Country Code</t>
   </si>
@@ -4398,6 +4398,9 @@
   </si>
   <si>
     <t>SAMP</t>
+  </si>
+  <si>
+    <t>LC</t>
   </si>
 </sst>
 </file>
@@ -4790,46 +4793,46 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F257" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I257" sqref="I257"/>
+      <selection pane="bottomRight" activeCell="I284" sqref="I284"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.6328125" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.6640625" customWidth="1"/>
     <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.26953125" customWidth="1"/>
-    <col min="22" max="22" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.21875" customWidth="1"/>
+    <col min="22" max="22" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="10" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4933,7 +4936,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -5013,7 +5016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -5084,7 +5087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -5158,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>24</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>28</v>
       </c>
@@ -5306,7 +5309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>32</v>
       </c>
@@ -5380,7 +5383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>51</v>
       </c>
@@ -5454,7 +5457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>533</v>
       </c>
@@ -5516,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>36</v>
       </c>
@@ -5587,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>40</v>
       </c>
@@ -5655,7 +5658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>31</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>44</v>
       </c>
@@ -5800,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>48</v>
       </c>
@@ -5871,7 +5874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>50</v>
       </c>
@@ -5945,7 +5948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>52</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>112</v>
       </c>
@@ -6090,7 +6093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>56</v>
       </c>
@@ -6158,7 +6161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>84</v>
       </c>
@@ -6232,7 +6235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>204</v>
       </c>
@@ -6318,7 +6321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>204</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>204</v>
       </c>
@@ -6478,7 +6481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>204</v>
       </c>
@@ -6558,7 +6561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>204</v>
       </c>
@@ -6638,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>204</v>
       </c>
@@ -6718,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>204</v>
       </c>
@@ -6798,7 +6801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>204</v>
       </c>
@@ -6878,7 +6881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>204</v>
       </c>
@@ -6958,7 +6961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>204</v>
       </c>
@@ -7038,7 +7041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>204</v>
       </c>
@@ -7118,7 +7121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>204</v>
       </c>
@@ -7198,7 +7201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>204</v>
       </c>
@@ -7278,7 +7281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>64</v>
       </c>
@@ -7352,7 +7355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>68</v>
       </c>
@@ -7429,7 +7432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>70</v>
       </c>
@@ -7500,7 +7503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>72</v>
       </c>
@@ -7586,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>76</v>
       </c>
@@ -7663,7 +7666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>96</v>
       </c>
@@ -7734,7 +7737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>100</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>854</v>
       </c>
@@ -7891,7 +7894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>108</v>
       </c>
@@ -7971,7 +7974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>116</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>120</v>
       </c>
@@ -8137,7 +8140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>124</v>
       </c>
@@ -8205,7 +8208,7 @@
         <v>31112</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>132</v>
       </c>
@@ -8279,7 +8282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>140</v>
       </c>
@@ -8365,7 +8368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>148</v>
       </c>
@@ -8451,7 +8454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>830</v>
       </c>
@@ -8513,7 +8516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>152</v>
       </c>
@@ -8590,7 +8593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>156</v>
       </c>
@@ -8667,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>344</v>
       </c>
@@ -8729,7 +8732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>446</v>
       </c>
@@ -8791,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>158</v>
       </c>
@@ -8856,7 +8859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>170</v>
       </c>
@@ -8930,7 +8933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>174</v>
       </c>
@@ -9004,7 +9007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>178</v>
       </c>
@@ -9090,7 +9093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>188</v>
       </c>
@@ -9164,7 +9167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>384</v>
       </c>
@@ -9247,7 +9250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>384</v>
       </c>
@@ -9327,7 +9330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>384</v>
       </c>
@@ -9407,7 +9410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>384</v>
       </c>
@@ -9487,7 +9490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>384</v>
       </c>
@@ -9567,7 +9570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>384</v>
       </c>
@@ -9647,7 +9650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>384</v>
       </c>
@@ -9727,7 +9730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>384</v>
       </c>
@@ -9807,7 +9810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>384</v>
       </c>
@@ -9887,7 +9890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>384</v>
       </c>
@@ -9967,7 +9970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>384</v>
       </c>
@@ -10047,7 +10050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>384</v>
       </c>
@@ -10127,7 +10130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>191</v>
       </c>
@@ -10201,7 +10204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>192</v>
       </c>
@@ -10275,7 +10278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>531</v>
       </c>
@@ -10337,7 +10340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>196</v>
       </c>
@@ -10408,7 +10411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>203</v>
       </c>
@@ -10482,7 +10485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>408</v>
       </c>
@@ -10553,7 +10556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>180</v>
       </c>
@@ -10639,7 +10642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>208</v>
       </c>
@@ -10710,7 +10713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>262</v>
       </c>
@@ -10784,7 +10787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>212</v>
       </c>
@@ -10849,7 +10852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>214</v>
       </c>
@@ -10929,7 +10932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>218</v>
       </c>
@@ -11009,7 +11012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>818</v>
       </c>
@@ -11083,7 +11086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>222</v>
       </c>
@@ -11163,7 +11166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>226</v>
       </c>
@@ -11243,7 +11246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>232</v>
       </c>
@@ -11323,7 +11326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>233</v>
       </c>
@@ -11394,7 +11397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>231</v>
       </c>
@@ -11480,7 +11483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>231</v>
       </c>
@@ -11560,7 +11563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>231</v>
       </c>
@@ -11640,7 +11643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>231</v>
       </c>
@@ -11720,7 +11723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>231</v>
       </c>
@@ -11800,7 +11803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>231</v>
       </c>
@@ -11880,7 +11883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>231</v>
       </c>
@@ -11960,7 +11963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>231</v>
       </c>
@@ -12040,7 +12043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>231</v>
       </c>
@@ -12120,7 +12123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>231</v>
       </c>
@@ -12200,7 +12203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>231</v>
       </c>
@@ -12280,7 +12283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>231</v>
       </c>
@@ -12360,7 +12363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>231</v>
       </c>
@@ -12440,7 +12443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>242</v>
       </c>
@@ -12514,7 +12517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>246</v>
       </c>
@@ -12582,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>250</v>
       </c>
@@ -12653,7 +12656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>254</v>
       </c>
@@ -12715,7 +12718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>258</v>
       </c>
@@ -12777,7 +12780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>266</v>
       </c>
@@ -12863,7 +12866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>270</v>
       </c>
@@ -12943,7 +12946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>268</v>
       </c>
@@ -13017,7 +13020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>276</v>
       </c>
@@ -13085,7 +13088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>288</v>
       </c>
@@ -13171,7 +13174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>300</v>
       </c>
@@ -13242,7 +13245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>308</v>
       </c>
@@ -13316,7 +13319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>312</v>
       </c>
@@ -13378,7 +13381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>316</v>
       </c>
@@ -13440,7 +13443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>320</v>
       </c>
@@ -13520,7 +13523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>324</v>
       </c>
@@ -13606,7 +13609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>624</v>
       </c>
@@ -13686,7 +13689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>328</v>
       </c>
@@ -13760,7 +13763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>332</v>
       </c>
@@ -13837,7 +13840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>332</v>
       </c>
@@ -13914,7 +13917,7 @@
       </c>
       <c r="AH119" s="3"/>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>332</v>
       </c>
@@ -13991,7 +13994,7 @@
       </c>
       <c r="AH120" s="3"/>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>332</v>
       </c>
@@ -14068,7 +14071,7 @@
       </c>
       <c r="AH121" s="3"/>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>332</v>
       </c>
@@ -14145,7 +14148,7 @@
       </c>
       <c r="AH122" s="3"/>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>332</v>
       </c>
@@ -14222,7 +14225,7 @@
       </c>
       <c r="AH123" s="3"/>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>332</v>
       </c>
@@ -14299,7 +14302,7 @@
       </c>
       <c r="AH124" s="3"/>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>332</v>
       </c>
@@ -14376,7 +14379,7 @@
       </c>
       <c r="AH125" s="3"/>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>332</v>
       </c>
@@ -14453,7 +14456,7 @@
       </c>
       <c r="AH126" s="3"/>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>332</v>
       </c>
@@ -14530,7 +14533,7 @@
       </c>
       <c r="AH127" s="3"/>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>332</v>
       </c>
@@ -14607,7 +14610,7 @@
       </c>
       <c r="AH128" s="3"/>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>340</v>
       </c>
@@ -14681,7 +14684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>348</v>
       </c>
@@ -14752,7 +14755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>352</v>
       </c>
@@ -14823,7 +14826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>356</v>
       </c>
@@ -14900,7 +14903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>356</v>
       </c>
@@ -14938,7 +14941,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>356</v>
       </c>
@@ -14976,7 +14979,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>356</v>
       </c>
@@ -15014,7 +15017,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>356</v>
       </c>
@@ -15052,7 +15055,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>356</v>
       </c>
@@ -15090,7 +15093,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="138" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>356</v>
       </c>
@@ -15128,7 +15131,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="139" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>356</v>
       </c>
@@ -15166,7 +15169,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="140" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>356</v>
       </c>
@@ -15204,7 +15207,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="141" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>356</v>
       </c>
@@ -15242,7 +15245,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="142" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>356</v>
       </c>
@@ -15280,7 +15283,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>356</v>
       </c>
@@ -15318,7 +15321,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="144" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>356</v>
       </c>
@@ -15356,7 +15359,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>356</v>
       </c>
@@ -15394,7 +15397,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>356</v>
       </c>
@@ -15432,7 +15435,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>356</v>
       </c>
@@ -15470,7 +15473,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>356</v>
       </c>
@@ -15508,7 +15511,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>356</v>
       </c>
@@ -15546,7 +15549,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>356</v>
       </c>
@@ -15584,7 +15587,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>356</v>
       </c>
@@ -15622,7 +15625,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>356</v>
       </c>
@@ -15660,7 +15663,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>356</v>
       </c>
@@ -15698,7 +15701,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>356</v>
       </c>
@@ -15736,7 +15739,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>356</v>
       </c>
@@ -15774,7 +15777,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>356</v>
       </c>
@@ -15812,7 +15815,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>356</v>
       </c>
@@ -15850,7 +15853,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>356</v>
       </c>
@@ -15888,7 +15891,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>356</v>
       </c>
@@ -15926,7 +15929,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>356</v>
       </c>
@@ -15964,7 +15967,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="161" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>356</v>
       </c>
@@ -16002,7 +16005,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="162" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>356</v>
       </c>
@@ -16040,7 +16043,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="163" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>356</v>
       </c>
@@ -16078,7 +16081,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="164" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>356</v>
       </c>
@@ -16116,7 +16119,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="165" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>356</v>
       </c>
@@ -16154,7 +16157,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="166" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>356</v>
       </c>
@@ -16192,7 +16195,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="167" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>356</v>
       </c>
@@ -16230,7 +16233,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="168" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>360</v>
       </c>
@@ -16310,7 +16313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>364</v>
       </c>
@@ -16381,7 +16384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>368</v>
       </c>
@@ -16452,7 +16455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>372</v>
       </c>
@@ -16523,7 +16526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>376</v>
       </c>
@@ -16591,7 +16594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>380</v>
       </c>
@@ -16662,7 +16665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>388</v>
       </c>
@@ -16733,7 +16736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>392</v>
       </c>
@@ -16801,7 +16804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>400</v>
       </c>
@@ -16875,7 +16878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>398</v>
       </c>
@@ -16946,7 +16949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>404</v>
       </c>
@@ -17032,7 +17035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>404</v>
       </c>
@@ -17112,7 +17115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>404</v>
       </c>
@@ -17192,7 +17195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>404</v>
       </c>
@@ -17272,7 +17275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>404</v>
       </c>
@@ -17352,7 +17355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>404</v>
       </c>
@@ -17432,7 +17435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>404</v>
       </c>
@@ -17512,7 +17515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>404</v>
       </c>
@@ -17592,7 +17595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>404</v>
       </c>
@@ -17672,7 +17675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>296</v>
       </c>
@@ -17743,7 +17746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A188" s="5">
         <v>412</v>
       </c>
@@ -17815,7 +17818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>414</v>
       </c>
@@ -17889,7 +17892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>417</v>
       </c>
@@ -17963,7 +17966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>418</v>
       </c>
@@ -18037,7 +18040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>428</v>
       </c>
@@ -18108,7 +18111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>422</v>
       </c>
@@ -18182,7 +18185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>426</v>
       </c>
@@ -18268,7 +18271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>430</v>
       </c>
@@ -18348,7 +18351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>434</v>
       </c>
@@ -18419,7 +18422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>440</v>
       </c>
@@ -18493,7 +18496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>442</v>
       </c>
@@ -18564,7 +18567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>450</v>
       </c>
@@ -18650,7 +18653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>454</v>
       </c>
@@ -18736,7 +18739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>458</v>
       </c>
@@ -18816,7 +18819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>462</v>
       </c>
@@ -18890,7 +18893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>466</v>
       </c>
@@ -18976,7 +18979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>470</v>
       </c>
@@ -19047,7 +19050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>474</v>
       </c>
@@ -19109,7 +19112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>478</v>
       </c>
@@ -19189,7 +19192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>480</v>
       </c>
@@ -19263,7 +19266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>175</v>
       </c>
@@ -19325,7 +19328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>484</v>
       </c>
@@ -19405,7 +19408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>583</v>
       </c>
@@ -19476,7 +19479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>496</v>
       </c>
@@ -19556,7 +19559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>499</v>
       </c>
@@ -19630,7 +19633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>504</v>
       </c>
@@ -19707,7 +19710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>508</v>
       </c>
@@ -19793,7 +19796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A215" s="3">
         <v>508</v>
       </c>
@@ -19873,7 +19876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A216" s="3">
         <v>508</v>
       </c>
@@ -19953,7 +19956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A217" s="3">
         <v>508</v>
       </c>
@@ -20033,7 +20036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A218" s="3">
         <v>508</v>
       </c>
@@ -20113,7 +20116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A219" s="3">
         <v>508</v>
       </c>
@@ -20193,7 +20196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A220" s="3">
         <v>508</v>
       </c>
@@ -20273,7 +20276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A221" s="3">
         <v>508</v>
       </c>
@@ -20353,7 +20356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A222" s="3">
         <v>508</v>
       </c>
@@ -20433,7 +20436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A223" s="3">
         <v>508</v>
       </c>
@@ -20513,7 +20516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A224" s="3">
         <v>508</v>
       </c>
@@ -20593,7 +20596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A225" s="3">
         <v>508</v>
       </c>
@@ -20673,7 +20676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>104</v>
       </c>
@@ -20753,7 +20756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>516</v>
       </c>
@@ -20839,7 +20842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>524</v>
       </c>
@@ -20919,7 +20922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>528</v>
       </c>
@@ -20990,7 +20993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>540</v>
       </c>
@@ -21052,7 +21055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>554</v>
       </c>
@@ -21123,7 +21126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>558</v>
       </c>
@@ -21197,7 +21200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>562</v>
       </c>
@@ -21283,7 +21286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>566</v>
       </c>
@@ -21366,7 +21369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A235" s="3">
         <v>566</v>
       </c>
@@ -21446,7 +21449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A236" s="3">
         <v>566</v>
       </c>
@@ -21526,7 +21529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A237" s="3">
         <v>566</v>
       </c>
@@ -21606,7 +21609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A238" s="3">
         <v>566</v>
       </c>
@@ -21686,7 +21689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A239" s="3">
         <v>566</v>
       </c>
@@ -21766,7 +21769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A240" s="3">
         <v>566</v>
       </c>
@@ -21846,7 +21849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A241" s="3">
         <v>566</v>
       </c>
@@ -21926,7 +21929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A242" s="3">
         <v>566</v>
       </c>
@@ -22006,7 +22009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A243" s="3">
         <v>566</v>
       </c>
@@ -22086,7 +22089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A244" s="3">
         <v>566</v>
       </c>
@@ -22166,7 +22169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A245" s="3">
         <v>566</v>
       </c>
@@ -22246,7 +22249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A246" s="3">
         <v>566</v>
       </c>
@@ -22326,7 +22329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A247" s="3">
         <v>566</v>
       </c>
@@ -22406,7 +22409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A248" s="3">
         <v>566</v>
       </c>
@@ -22486,7 +22489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A249" s="3">
         <v>566</v>
       </c>
@@ -22566,7 +22569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A250" s="3">
         <v>566</v>
       </c>
@@ -22646,7 +22649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A251" s="3">
         <v>566</v>
       </c>
@@ -22726,7 +22729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A252" s="3">
         <v>566</v>
       </c>
@@ -22806,7 +22809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A253" s="3">
         <v>566</v>
       </c>
@@ -22886,7 +22889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A254" s="3">
         <v>566</v>
       </c>
@@ -22966,7 +22969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A255" s="3">
         <v>566</v>
       </c>
@@ -23046,7 +23049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A256" s="3">
         <v>566</v>
       </c>
@@ -23126,7 +23129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A257" s="3">
         <v>566</v>
       </c>
@@ -23206,7 +23209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A258" s="3">
         <v>566</v>
       </c>
@@ -23286,7 +23289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A259" s="3">
         <v>566</v>
       </c>
@@ -23366,7 +23369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A260" s="3">
         <v>566</v>
       </c>
@@ -23446,7 +23449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A261" s="3">
         <v>566</v>
       </c>
@@ -23526,7 +23529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A262" s="3">
         <v>566</v>
       </c>
@@ -23606,7 +23609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A263" s="3">
         <v>566</v>
       </c>
@@ -23686,7 +23689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A264" s="3">
         <v>566</v>
       </c>
@@ -23766,7 +23769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A265" s="3">
         <v>566</v>
       </c>
@@ -23846,7 +23849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A266" s="3">
         <v>566</v>
       </c>
@@ -23926,7 +23929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A267" s="3">
         <v>566</v>
       </c>
@@ -24006,7 +24009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A268" s="3">
         <v>566</v>
       </c>
@@ -24086,7 +24089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A269" s="3">
         <v>566</v>
       </c>
@@ -24166,7 +24169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A270" s="3">
         <v>566</v>
       </c>
@@ -24246,7 +24249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A271" s="3">
         <v>566</v>
       </c>
@@ -24326,7 +24329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>578</v>
       </c>
@@ -24394,7 +24397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>275</v>
       </c>
@@ -24462,7 +24465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>512</v>
       </c>
@@ -24533,7 +24536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>586</v>
       </c>
@@ -24613,7 +24616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>591</v>
       </c>
@@ -24693,7 +24696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>598</v>
       </c>
@@ -24773,7 +24776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>600</v>
       </c>
@@ -24853,7 +24856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>604</v>
       </c>
@@ -24933,7 +24936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>608</v>
       </c>
@@ -25013,7 +25016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>616</v>
       </c>
@@ -25084,7 +25087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>620</v>
       </c>
@@ -25155,7 +25158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>630</v>
       </c>
@@ -25217,7 +25220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>634</v>
       </c>
@@ -25291,7 +25294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>410</v>
       </c>
@@ -25362,7 +25365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>498</v>
       </c>
@@ -25436,7 +25439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A287" s="3">
         <v>498</v>
       </c>
@@ -25512,7 +25515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A288" s="3">
         <v>498</v>
       </c>
@@ -25588,7 +25591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>638</v>
       </c>
@@ -25650,7 +25653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>642</v>
       </c>
@@ -25724,7 +25727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>643</v>
       </c>
@@ -25795,7 +25798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>646</v>
       </c>
@@ -25881,7 +25884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>659</v>
       </c>
@@ -25952,7 +25955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>662</v>
       </c>
@@ -26023,7 +26026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>670</v>
       </c>
@@ -26094,7 +26097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>882</v>
       </c>
@@ -26165,7 +26168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>5733</v>
       </c>
@@ -26182,10 +26185,10 @@
         <v>277</v>
       </c>
       <c r="G297">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H297" t="s">
-        <v>277</v>
+        <v>1458</v>
       </c>
       <c r="I297" s="3" t="s">
         <v>521</v>
@@ -26236,7 +26239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>678</v>
       </c>
@@ -26310,7 +26313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>682</v>
       </c>
@@ -26381,7 +26384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>686</v>
       </c>
@@ -26467,7 +26470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>688</v>
       </c>
@@ -26541,7 +26544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>690</v>
       </c>
@@ -26609,7 +26612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>694</v>
       </c>
@@ -26695,7 +26698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>702</v>
       </c>
@@ -26766,7 +26769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>703</v>
       </c>
@@ -26840,7 +26843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>705</v>
       </c>
@@ -26914,7 +26917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>90</v>
       </c>
@@ -26985,7 +26988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>706</v>
       </c>
@@ -27062,7 +27065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>710</v>
       </c>
@@ -27148,7 +27151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>728</v>
       </c>
@@ -27228,7 +27231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>724</v>
       </c>
@@ -27296,7 +27299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>144</v>
       </c>
@@ -27370,7 +27373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>729</v>
       </c>
@@ -27444,7 +27447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>740</v>
       </c>
@@ -27515,7 +27518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>748</v>
       </c>
@@ -27601,7 +27604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>752</v>
       </c>
@@ -27669,7 +27672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>756</v>
       </c>
@@ -27737,7 +27740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>760</v>
       </c>
@@ -27811,7 +27814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>762</v>
       </c>
@@ -27885,7 +27888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>807</v>
       </c>
@@ -27959,7 +27962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>764</v>
       </c>
@@ -28039,7 +28042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>626</v>
       </c>
@@ -28113,7 +28116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>768</v>
       </c>
@@ -28199,7 +28202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A324" s="3">
         <v>768</v>
       </c>
@@ -28279,7 +28282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A325" s="3">
         <v>768</v>
       </c>
@@ -28359,7 +28362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A326" s="3">
         <v>768</v>
       </c>
@@ -28439,7 +28442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A327" s="3">
         <v>768</v>
       </c>
@@ -28519,7 +28522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A328" s="3">
         <v>768</v>
       </c>
@@ -28599,7 +28602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A329" s="3">
         <v>768</v>
       </c>
@@ -28679,7 +28682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>776</v>
       </c>
@@ -28750,7 +28753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>780</v>
       </c>
@@ -28824,7 +28827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>788</v>
       </c>
@@ -28901,7 +28904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>792</v>
       </c>
@@ -28972,7 +28975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>795</v>
       </c>
@@ -29043,7 +29046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>800</v>
       </c>
@@ -29129,7 +29132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A336" s="3">
         <v>800</v>
       </c>
@@ -29209,7 +29212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A337" s="3">
         <v>800</v>
       </c>
@@ -29289,7 +29292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A338" s="3">
         <v>800</v>
       </c>
@@ -29369,7 +29372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A339" s="3">
         <v>800</v>
       </c>
@@ -29449,7 +29452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A340" s="3">
         <v>800</v>
       </c>
@@ -29529,7 +29532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A341" s="3">
         <v>800</v>
       </c>
@@ -29609,7 +29612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A342" s="3">
         <v>800</v>
       </c>
@@ -29689,7 +29692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A343" s="3">
         <v>800</v>
       </c>
@@ -29769,7 +29772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A344" s="3">
         <v>800</v>
       </c>
@@ -29849,7 +29852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>804</v>
       </c>
@@ -29920,7 +29923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>784</v>
       </c>
@@ -29991,7 +29994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>826</v>
       </c>
@@ -30059,7 +30062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>834</v>
       </c>
@@ -30145,7 +30148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A349" s="3">
         <v>834</v>
       </c>
@@ -30225,7 +30228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A350" s="3">
         <v>834</v>
       </c>
@@ -30305,7 +30308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A351" s="3">
         <v>834</v>
       </c>
@@ -30385,7 +30388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A352" s="3">
         <v>834</v>
       </c>
@@ -30465,7 +30468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A353" s="3">
         <v>834</v>
       </c>
@@ -30545,7 +30548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A354" s="3">
         <v>834</v>
       </c>
@@ -30625,7 +30628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A355" s="3">
         <v>834</v>
       </c>
@@ -30705,7 +30708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A356" s="3">
         <v>834</v>
       </c>
@@ -30785,7 +30788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A357" s="3">
         <v>834</v>
       </c>
@@ -30865,7 +30868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A358" s="3">
         <v>834</v>
       </c>
@@ -30945,7 +30948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A359" s="3">
         <v>834</v>
       </c>
@@ -31025,7 +31028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A360" s="3">
         <v>834</v>
       </c>
@@ -31105,7 +31108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A361" s="3">
         <v>834</v>
       </c>
@@ -31185,7 +31188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A362" s="3">
         <v>834</v>
       </c>
@@ -31265,7 +31268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A363" s="3">
         <v>834</v>
       </c>
@@ -31345,7 +31348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A364" s="3">
         <v>834</v>
       </c>
@@ -31425,7 +31428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A365" s="3">
         <v>834</v>
       </c>
@@ -31505,7 +31508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A366" s="3">
         <v>834</v>
       </c>
@@ -31585,7 +31588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A367" s="3">
         <v>834</v>
       </c>
@@ -31665,7 +31668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A368" s="3">
         <v>834</v>
       </c>
@@ -31745,7 +31748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A369" s="3">
         <v>834</v>
       </c>
@@ -31825,7 +31828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A370" s="3">
         <v>834</v>
       </c>
@@ -31905,7 +31908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A371" s="3">
         <v>834</v>
       </c>
@@ -31985,7 +31988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A372" s="3">
         <v>834</v>
       </c>
@@ -32065,7 +32068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A373" s="3">
         <v>834</v>
       </c>
@@ -32145,7 +32148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A374" s="3">
         <v>834</v>
       </c>
@@ -32225,7 +32228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A375" s="3">
         <v>834</v>
       </c>
@@ -32305,7 +32308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>840</v>
       </c>
@@ -32370,7 +32373,7 @@
         <v>31112</v>
       </c>
     </row>
-    <row r="377" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>850</v>
       </c>
@@ -32429,7 +32432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>858</v>
       </c>
@@ -32503,7 +32506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>860</v>
       </c>
@@ -32574,7 +32577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>548</v>
       </c>
@@ -32642,7 +32645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>862</v>
       </c>
@@ -32713,7 +32716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>704</v>
       </c>
@@ -32790,7 +32793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>732</v>
       </c>
@@ -32852,7 +32855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>887</v>
       </c>
@@ -32926,7 +32929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>894</v>
       </c>
@@ -33012,7 +33015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A386" s="3">
         <v>894</v>
       </c>
@@ -33092,7 +33095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A387" s="3">
         <v>894</v>
       </c>
@@ -33172,7 +33175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A388" s="3">
         <v>894</v>
       </c>
@@ -33252,7 +33255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A389" s="3">
         <v>894</v>
       </c>
@@ -33332,7 +33335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A390" s="3">
         <v>894</v>
       </c>
@@ -33412,7 +33415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A391" s="3">
         <v>894</v>
       </c>
@@ -33492,7 +33495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A392" s="3">
         <v>894</v>
       </c>
@@ -33572,7 +33575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A393" s="3">
         <v>894</v>
       </c>
@@ -33652,7 +33655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A394" s="3">
         <v>894</v>
       </c>
@@ -33732,7 +33735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A395" s="3">
         <v>894</v>
       </c>
@@ -33812,7 +33815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>716</v>
       </c>
@@ -33898,7 +33901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A397" s="3">
         <v>716</v>
       </c>
@@ -33978,7 +33981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A398" s="3">
         <v>716</v>
       </c>
@@ -34058,7 +34061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A399" s="3">
         <v>716</v>
       </c>
@@ -34138,7 +34141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A400" s="3">
         <v>716</v>
       </c>
@@ -34218,7 +34221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A401" s="3">
         <v>716</v>
       </c>
@@ -34298,7 +34301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A402" s="3">
         <v>716</v>
       </c>
@@ -34378,7 +34381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A403" s="3">
         <v>716</v>
       </c>
@@ -34458,7 +34461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A404" s="3">
         <v>716</v>
       </c>
@@ -34538,7 +34541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A405" s="3">
         <v>716</v>
       </c>
@@ -34618,7 +34621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A406" s="3">
         <v>716</v>
       </c>
@@ -34711,14 +34714,14 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="52.1796875" customWidth="1"/>
-    <col min="3" max="4" width="73.26953125" customWidth="1"/>
+    <col min="2" max="2" width="52.21875" customWidth="1"/>
+    <col min="3" max="4" width="73.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>668</v>
       </c>
@@ -34732,7 +34735,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>903</v>
       </c>
@@ -34746,7 +34749,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>935</v>
       </c>
@@ -34760,7 +34763,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>927</v>
       </c>
@@ -34774,7 +34777,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>915</v>
       </c>
@@ -34788,7 +34791,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>916</v>
       </c>
@@ -34802,7 +34805,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5500</v>
       </c>
@@ -34816,7 +34819,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>910</v>
       </c>
@@ -34830,7 +34833,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1832</v>
       </c>
@@ -34844,7 +34847,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>906</v>
       </c>
@@ -34858,7 +34861,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>923</v>
       </c>
@@ -34872,7 +34875,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>908</v>
       </c>
@@ -34886,7 +34889,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1829</v>
       </c>
@@ -34900,7 +34903,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1503</v>
       </c>
@@ -34914,7 +34917,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>904</v>
       </c>
@@ -34928,7 +34931,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>941</v>
       </c>
@@ -34942,7 +34945,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>902</v>
       </c>
@@ -34956,7 +34959,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>948</v>
       </c>
@@ -34970,7 +34973,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>934</v>
       </c>
@@ -34984,7 +34987,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1501</v>
       </c>
@@ -34998,7 +35001,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1500</v>
       </c>
@@ -35012,7 +35015,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>928</v>
       </c>
@@ -35026,7 +35029,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>954</v>
       </c>
@@ -35040,7 +35043,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>911</v>
       </c>
@@ -35054,7 +35057,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1517</v>
       </c>
@@ -35068,7 +35071,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>901</v>
       </c>
@@ -35082,7 +35085,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1518</v>
       </c>
@@ -35096,7 +35099,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>912</v>
       </c>
@@ -35110,7 +35113,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>905</v>
       </c>
@@ -35124,7 +35127,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1833</v>
       </c>
@@ -35138,7 +35141,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>924</v>
       </c>
@@ -35152,7 +35155,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1835</v>
       </c>
@@ -35166,7 +35169,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>909</v>
       </c>
@@ -35180,7 +35183,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>957</v>
       </c>
@@ -35194,7 +35197,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>931</v>
       </c>
@@ -35208,7 +35211,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5501</v>
       </c>
@@ -35222,7 +35225,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1831</v>
       </c>
@@ -35236,7 +35239,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>920</v>
       </c>
@@ -35250,7 +35253,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>913</v>
       </c>
@@ -35264,7 +35267,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>925</v>
       </c>
@@ -35278,7 +35281,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1834</v>
       </c>
@@ -35292,7 +35295,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1502</v>
       </c>
@@ -35306,7 +35309,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>914</v>
       </c>
@@ -35320,7 +35323,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>922</v>
       </c>
@@ -35334,7 +35337,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>926</v>
       </c>
@@ -35348,7 +35351,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>900</v>
       </c>
@@ -35374,13 +35377,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="52.26953125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="52.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>703</v>
       </c>
@@ -35388,7 +35391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>31100</v>
       </c>
@@ -35396,7 +35399,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>31101</v>
       </c>
@@ -35404,7 +35407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>31102</v>
       </c>
@@ -35412,7 +35415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>31103</v>
       </c>
@@ -35420,7 +35423,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>31104</v>
       </c>
@@ -35428,7 +35431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>31105</v>
       </c>
@@ -35436,7 +35439,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>31106</v>
       </c>
@@ -35444,7 +35447,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>31107</v>
       </c>
@@ -35452,7 +35455,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>31108</v>
       </c>
@@ -35460,7 +35463,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>31109</v>
       </c>
@@ -35468,7 +35471,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>31110</v>
       </c>
@@ -35476,7 +35479,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>31111</v>
       </c>
@@ -35484,7 +35487,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>31112</v>
       </c>
@@ -35492,7 +35495,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>31113</v>
       </c>
@@ -35500,7 +35503,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>31114</v>
       </c>
@@ -35508,7 +35511,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>31115</v>
       </c>
@@ -35516,7 +35519,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>31116</v>
       </c>
@@ -35524,7 +35527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>31117</v>
       </c>
@@ -35532,7 +35535,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>31118</v>
       </c>
@@ -35540,7 +35543,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>31119</v>
       </c>
@@ -35548,7 +35551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>31120</v>
       </c>
@@ -35568,9 +35571,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>670</v>
       </c>
@@ -35578,7 +35581,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>672</v>
       </c>
@@ -35658,7 +35661,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>686</v>
       </c>
@@ -35738,7 +35741,7 @@
         <v>0.199826844</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>687</v>
       </c>
@@ -35818,7 +35821,7 @@
         <v>0.25524005999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>688</v>
       </c>
@@ -35898,7 +35901,7 @@
         <v>0.20412380699999999</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>689</v>
       </c>
@@ -35978,7 +35981,7 @@
         <v>0.29957267999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>690</v>
       </c>
@@ -36058,7 +36061,7 @@
         <v>0.26680348199999998</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -36138,7 +36141,7 @@
         <v>0.23617002600000001</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -36218,7 +36221,7 @@
         <v>0.28607152800000002</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>691</v>
       </c>
@@ -36298,7 +36301,7 @@
         <v>0.25205312499999999</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>692</v>
       </c>
@@ -36378,7 +36381,7 @@
         <v>0.24749605999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>693</v>
       </c>
@@ -36458,7 +36461,7 @@
         <v>0.23831311399999999</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>694</v>
       </c>
@@ -36538,7 +36541,7 @@
         <v>0.26037552000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>695</v>
       </c>
@@ -36618,7 +36621,7 @@
         <v>0.249594433</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>696</v>
       </c>
@@ -36698,7 +36701,7 @@
         <v>0.257790136</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>697</v>
       </c>
@@ -36778,7 +36781,7 @@
         <v>0.26470371500000001</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>698</v>
       </c>
@@ -36858,7 +36861,7 @@
         <v>0.298197449</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>144</v>
       </c>
@@ -36938,7 +36941,7 @@
         <v>0.24057669000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>245</v>
       </c>
@@ -37018,7 +37021,7 @@
         <v>0.319881423</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>699</v>
       </c>
@@ -37098,7 +37101,7 @@
         <v>0.30209310099999998</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>700</v>
       </c>
@@ -37178,7 +37181,7 @@
         <v>0.30532294700000001</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>701</v>
       </c>
@@ -37258,7 +37261,7 @@
         <v>0.28461773499999998</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>702</v>
       </c>
@@ -37351,15 +37354,15 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="22.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>749</v>
       </c>
@@ -37373,7 +37376,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>753</v>
       </c>
@@ -37394,6 +37397,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016926C673858A24ABD1F0F68A585E074" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1931556e2b88a0a7c72249bbb83367d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c9bee02-199a-488a-b277-ba7f212fbf06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="613c55408f90ae378c42e0f4853623d2" ns3:_="">
     <xsd:import namespace="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
@@ -37595,35 +37613,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC31D53-F79F-4F2D-98CF-E26337BE3FD1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37645,9 +37638,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC31D53-F79F-4F2D-98CF-E26337BE3FD1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated currency column for Sample country, since the currency that shows in the client comes from that.
</commit_message>
<xml_diff>
--- a/SourceData/globals/GBModData.xlsx
+++ b/SourceData/globals/GBModData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1424D40-CB90-4576-BDB0-A23C534A0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A221A0-2510-406D-98CE-E7D0B663A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryMaster" sheetId="1" r:id="rId1"/>
@@ -4790,10 +4790,10 @@
   <dimension ref="A1:AH406"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F257" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F281" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I284" sqref="I284"/>
+      <selection pane="bottomRight" activeCell="H300" sqref="H300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26182,7 +26182,7 @@
         <v>0</v>
       </c>
       <c r="F297" t="s">
-        <v>277</v>
+        <v>1458</v>
       </c>
       <c r="G297">
         <v>100</v>
@@ -37397,21 +37397,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016926C673858A24ABD1F0F68A585E074" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1931556e2b88a0a7c72249bbb83367d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c9bee02-199a-488a-b277-ba7f212fbf06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="613c55408f90ae378c42e0f4853623d2" ns3:_="">
     <xsd:import namespace="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
@@ -37613,10 +37598,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC31D53-F79F-4F2D-98CF-E26337BE3FD1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37638,19 +37648,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDC31D53-F79F-4F2D-98CF-E26337BE3FD1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated surveys for LiST
</commit_message>
<xml_diff>
--- a/SourceData/globals/GBModData.xlsx
+++ b/SourceData/globals/GBModData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3903" uniqueCount="1459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3903" uniqueCount="1460">
   <si>
     <t>Country Code</t>
   </si>
@@ -4065,9 +4065,6 @@
     <t>UNAIDS 2023</t>
   </si>
   <si>
-    <t>MICS 2000, MICS 2010, DHS 2015</t>
-  </si>
-  <si>
     <t>RHS 2002, MICS 2005, DHS 2008, DHS 2017</t>
   </si>
   <si>
@@ -4095,9 +4092,6 @@
     <t>MICS 2005, MICS 2006, MICS 2011, MICS 2012, MICS 2015</t>
   </si>
   <si>
-    <t>DHS 1996, DHS 2001, DHS 2006, DHS 2011, MICS 2014, DHS 2017</t>
-  </si>
-  <si>
     <t>DHS 1998, MICS 2000, DHS 2003, DHS 2008, NSS 2016</t>
   </si>
   <si>
@@ -4110,9 +4104,6 @@
     <t>DHS 1996, NSS 2006, UNICEF SOWC 2009-2013 2009, NSS 2013, NSS 2019</t>
   </si>
   <si>
-    <t>DHS 1998, DHS 2003, MICS 2006, DHS 2010, MIS 2014</t>
-  </si>
-  <si>
     <t>MICS 2000, MICS 2005, DHS 2010, MIS 2012, DHS 2016</t>
   </si>
   <si>
@@ -4131,9 +4122,6 @@
     <t>DHS 1996, MICS 2000, DHS 2004, DHS 2005, MICS 2010, DHS 2014, MICS 2019</t>
   </si>
   <si>
-    <t>DHS 1996, MICS 2000, DHS 2012</t>
-  </si>
-  <si>
     <t>DHS 2005, DHS 2011, MICS 2014</t>
   </si>
   <si>
@@ -4143,9 +4131,6 @@
     <t>MICS 2011, MICS 2018</t>
   </si>
   <si>
-    <t>DHS 1998, MICS 2000, AIS 2005, MICS 2006, DHS 2011, MICS 2016</t>
-  </si>
-  <si>
     <t>MICS 2006, MICS 2010, MICS 2014, MICS 2019</t>
   </si>
   <si>
@@ -4185,9 +4170,6 @@
     <t>MICS 2005, MICS 2018</t>
   </si>
   <si>
-    <t>DHS 1998, DHS 2003, MICS 2006, DHS 2008, MICS 2011, DHS 2014, MICS 2017</t>
-  </si>
-  <si>
     <t>DHS 1998, RHS 2002, RHS 2008, DHS 2014</t>
   </si>
   <si>
@@ -4302,9 +4284,6 @@
     <t>RHS 1998, RHS 2004, RHS 2008, MICS 2016</t>
   </si>
   <si>
-    <t>DHS 1996, DHS 2000, DHS 2004, DHS 2005, DHS 2006, DHS 2007, DHS 2008, DHS 2009, DHS 2010, DHS 2011, DHS 2012, DHS 2013, DHS 2014, DHS 2015, DHS 2016, DHS 2017, DHS 2018, DHS 2019, DHS 2020, DHS 2021</t>
-  </si>
-  <si>
     <t>DHS 1998, MICS 2000, DHS 2003, DHS 2008, DHS 2013, DHS 2017, DHS 2022</t>
   </si>
   <si>
@@ -4344,21 +4323,12 @@
     <t>MICS 2006, MICS 2010, MICS 2018</t>
   </si>
   <si>
-    <t>MICS 2000, DHS 2006, MICS 2010, MICS 2014</t>
-  </si>
-  <si>
     <t>MICS 2000, MICS 2005, DHS 2012, DHS 2017</t>
   </si>
   <si>
-    <t>DHS 1996, DHS 1999, DHS 2004, DHS 2010, DHS 2015</t>
-  </si>
-  <si>
     <t>MICS 2005, MICS 2011, MICS 2018</t>
   </si>
   <si>
-    <t>MICS 2005, MICS 2012, MICS 2015, MICS 2019</t>
-  </si>
-  <si>
     <t>DHS 1998, MICS 2006, MICS 2010, DHS 2013, MICS 2017</t>
   </si>
   <si>
@@ -4386,9 +4356,6 @@
     <t>DHS 1997, MICS 2000, DHS 2002, MICS 2006, MICS 2010, MICS 2013, MICS 2020</t>
   </si>
   <si>
-    <t>DHS 1997, MICS 2006, DHS 2013</t>
-  </si>
-  <si>
     <t>DHS 1996, MICS 1999, DHS 2001, DHS 2007, DHS 2013, DHS 2018</t>
   </si>
   <si>
@@ -4399,6 +4366,42 @@
   </si>
   <si>
     <t>LC</t>
+  </si>
+  <si>
+    <t>MICS 2000, MICS 2010, DHS 2015, MICS 2022</t>
+  </si>
+  <si>
+    <t>DHS 1996, DHS 2001, DHS 2006, DHS 2011, MICS 2014, DHS 2017, MICS 2021</t>
+  </si>
+  <si>
+    <t>DHS 1998, DHS 2003, MICS 2006, DHS 2010, MIS 2014, DHS 2021</t>
+  </si>
+  <si>
+    <t>DHS 1996, MICS 2000, DHS 2012, MICS 2022</t>
+  </si>
+  <si>
+    <t>DHS 1998, MICS 2000, AIS 2005, MICS 2006, DHS 2011, MICS 2016, DHS 2021</t>
+  </si>
+  <si>
+    <t>DHS 1998, DHS 2003, MICS 2006, DHS 2008, MICS 2011, DHS 2014, MICS 2017, DHS 2022</t>
+  </si>
+  <si>
+    <t>DHS 1996, DHS 2000, DHS 2004, DHS 2005, DHS 2006, DHS 2007, DHS 2008, DHS 2009, DHS 2010, DHS 2011, DHS 2012, DHS 2013, DHS 2014, DHS 2015, DHS 2016, DHS 2017, DHS 2018, DHS 2019, DHS 2020, DHS 2021, DHS 2022</t>
+  </si>
+  <si>
+    <t>MICS 2000, DHS 2006, MICS 2010, MICS 2014, MICS 2021</t>
+  </si>
+  <si>
+    <t>DHS 1996, DHS 1999, DHS 2004, DHS 2010, DHS 2015, DHS 2022</t>
+  </si>
+  <si>
+    <t>MICS 2005, MICS 2012, MICS 2015, MICS 2019, MICS 2022</t>
+  </si>
+  <si>
+    <t>MICS 2006, MICS 2011, MICS 2022</t>
+  </si>
+  <si>
+    <t>DHS 1997, MICS 2006, DHS 2013, MICS 2022</t>
   </si>
 </sst>
 </file>
@@ -4998,7 +5001,7 @@
         <v>1221</v>
       </c>
       <c r="X2" t="s">
-        <v>1347</v>
+        <v>1448</v>
       </c>
       <c r="AA2" t="s">
         <v>966</v>
@@ -5072,7 +5075,7 @@
         <v>1222</v>
       </c>
       <c r="X3" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="AE3" t="s">
         <v>708</v>
@@ -5143,7 +5146,7 @@
         <v>1223</v>
       </c>
       <c r="X4" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="AA4" t="s">
         <v>966</v>
@@ -5220,7 +5223,7 @@
         <v>1224</v>
       </c>
       <c r="X5" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="AA5" t="s">
         <v>966</v>
@@ -5365,7 +5368,7 @@
         <v>1226</v>
       </c>
       <c r="X7" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="AA7" t="s">
         <v>966</v>
@@ -5439,7 +5442,7 @@
         <v>1227</v>
       </c>
       <c r="X8" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="AA8" t="s">
         <v>966</v>
@@ -5711,7 +5714,7 @@
         <v>1228</v>
       </c>
       <c r="X12" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="AA12" t="s">
         <v>966</v>
@@ -5930,7 +5933,7 @@
         <v>1229</v>
       </c>
       <c r="X15" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="AA15" t="s">
         <v>966</v>
@@ -6075,7 +6078,7 @@
         <v>1231</v>
       </c>
       <c r="X17" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="AA17" t="s">
         <v>966</v>
@@ -6217,7 +6220,7 @@
         <v>1232</v>
       </c>
       <c r="X19" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="AA19" t="s">
         <v>966</v>
@@ -6300,7 +6303,7 @@
         <v>1233</v>
       </c>
       <c r="X20" t="s">
-        <v>1357</v>
+        <v>1449</v>
       </c>
       <c r="AA20" t="s">
         <v>966</v>
@@ -7417,7 +7420,7 @@
         <v>1235</v>
       </c>
       <c r="X34" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="AA34" t="s">
         <v>966</v>
@@ -7485,7 +7488,7 @@
         <v>1236</v>
       </c>
       <c r="X35" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="AA35" t="s">
         <v>759</v>
@@ -7568,7 +7571,7 @@
         <v>759</v>
       </c>
       <c r="X36" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="AA36" t="s">
         <v>966</v>
@@ -7648,7 +7651,7 @@
         <v>1237</v>
       </c>
       <c r="X37" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="AA37" t="s">
         <v>966</v>
@@ -7873,7 +7876,7 @@
         <v>1240</v>
       </c>
       <c r="X40" t="s">
-        <v>1362</v>
+        <v>1450</v>
       </c>
       <c r="AA40" t="s">
         <v>966</v>
@@ -7953,7 +7956,7 @@
         <v>1241</v>
       </c>
       <c r="X41" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="AA41" t="s">
         <v>966</v>
@@ -8036,7 +8039,7 @@
         <v>1242</v>
       </c>
       <c r="X42" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="AA42" t="s">
         <v>966</v>
@@ -8119,7 +8122,7 @@
         <v>1243</v>
       </c>
       <c r="X43" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="AA43" t="s">
         <v>966</v>
@@ -8267,7 +8270,7 @@
         <v>1244</v>
       </c>
       <c r="X45" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="AA45" t="s">
         <v>966</v>
@@ -8347,7 +8350,7 @@
         <v>1245</v>
       </c>
       <c r="X46" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="AA46" t="s">
         <v>966</v>
@@ -8433,7 +8436,7 @@
         <v>1246</v>
       </c>
       <c r="X47" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="AA47" t="s">
         <v>966</v>
@@ -8915,7 +8918,7 @@
         <v>1249</v>
       </c>
       <c r="X54" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="AA54" t="s">
         <v>966</v>
@@ -8989,7 +8992,7 @@
         <v>1250</v>
       </c>
       <c r="X55" t="s">
-        <v>1369</v>
+        <v>1451</v>
       </c>
       <c r="AA55" t="s">
         <v>759</v>
@@ -9072,7 +9075,7 @@
         <v>1251</v>
       </c>
       <c r="X56" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="AA56" t="s">
         <v>966</v>
@@ -9149,7 +9152,7 @@
         <v>1252</v>
       </c>
       <c r="X57" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="AA57" t="s">
         <v>966</v>
@@ -9232,7 +9235,7 @@
         <v>1253</v>
       </c>
       <c r="X58" t="s">
-        <v>1373</v>
+        <v>1452</v>
       </c>
       <c r="AA58" t="s">
         <v>966</v>
@@ -10260,7 +10263,7 @@
         <v>1255</v>
       </c>
       <c r="X71" t="s">
-        <v>1374</v>
+        <v>1369</v>
       </c>
       <c r="AA71" t="s">
         <v>966</v>
@@ -10538,7 +10541,7 @@
         <v>1257</v>
       </c>
       <c r="X75" t="s">
-        <v>1375</v>
+        <v>1370</v>
       </c>
       <c r="AA75" t="s">
         <v>966</v>
@@ -10621,7 +10624,7 @@
         <v>1258</v>
       </c>
       <c r="X76" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="AA76" t="s">
         <v>966</v>
@@ -10914,7 +10917,7 @@
         <v>1260</v>
       </c>
       <c r="X80" t="s">
-        <v>1376</v>
+        <v>1371</v>
       </c>
       <c r="AA80" t="s">
         <v>966</v>
@@ -10994,7 +10997,7 @@
         <v>1261</v>
       </c>
       <c r="X81" t="s">
-        <v>1377</v>
+        <v>1372</v>
       </c>
       <c r="AA81" t="s">
         <v>966</v>
@@ -11065,7 +11068,7 @@
         <v>1262</v>
       </c>
       <c r="X82" t="s">
-        <v>1378</v>
+        <v>1373</v>
       </c>
       <c r="AA82" t="s">
         <v>966</v>
@@ -11148,7 +11151,7 @@
         <v>1263</v>
       </c>
       <c r="X83" t="s">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="AA83" t="s">
         <v>966</v>
@@ -11225,7 +11228,7 @@
         <v>1264</v>
       </c>
       <c r="X84" t="s">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="AA84" t="s">
         <v>966</v>
@@ -11305,7 +11308,7 @@
         <v>1265</v>
       </c>
       <c r="X85" t="s">
-        <v>1381</v>
+        <v>1376</v>
       </c>
       <c r="AA85" t="s">
         <v>966</v>
@@ -11462,7 +11465,7 @@
         <v>1266</v>
       </c>
       <c r="X87" t="s">
-        <v>1382</v>
+        <v>1377</v>
       </c>
       <c r="AA87" t="s">
         <v>966</v>
@@ -12499,7 +12502,7 @@
         <v>1267</v>
       </c>
       <c r="X100" t="s">
-        <v>1383</v>
+        <v>1378</v>
       </c>
       <c r="AA100" t="s">
         <v>966</v>
@@ -12845,7 +12848,7 @@
         <v>1268</v>
       </c>
       <c r="X105" t="s">
-        <v>1384</v>
+        <v>1379</v>
       </c>
       <c r="AA105" t="s">
         <v>966</v>
@@ -12925,7 +12928,7 @@
         <v>1269</v>
       </c>
       <c r="X106" t="s">
-        <v>1385</v>
+        <v>1380</v>
       </c>
       <c r="AA106" t="s">
         <v>966</v>
@@ -13002,7 +13005,7 @@
         <v>1270</v>
       </c>
       <c r="X107" t="s">
-        <v>1386</v>
+        <v>1381</v>
       </c>
       <c r="AA107" t="s">
         <v>966</v>
@@ -13153,7 +13156,7 @@
         <v>1271</v>
       </c>
       <c r="X109" t="s">
-        <v>1387</v>
+        <v>1453</v>
       </c>
       <c r="AA109" t="s">
         <v>966</v>
@@ -13505,7 +13508,7 @@
         <v>1272</v>
       </c>
       <c r="X114" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="AA114" t="s">
         <v>966</v>
@@ -13588,7 +13591,7 @@
         <v>1273</v>
       </c>
       <c r="X115" t="s">
-        <v>1389</v>
+        <v>1383</v>
       </c>
       <c r="AA115" t="s">
         <v>966</v>
@@ -13668,7 +13671,7 @@
         <v>1274</v>
       </c>
       <c r="X116" t="s">
-        <v>1390</v>
+        <v>1384</v>
       </c>
       <c r="AA116" t="s">
         <v>966</v>
@@ -13745,7 +13748,7 @@
         <v>1275</v>
       </c>
       <c r="X117" t="s">
-        <v>1391</v>
+        <v>1385</v>
       </c>
       <c r="AA117" t="s">
         <v>966</v>
@@ -13822,7 +13825,7 @@
         <v>1276</v>
       </c>
       <c r="X118" t="s">
-        <v>1392</v>
+        <v>1386</v>
       </c>
       <c r="AA118" t="s">
         <v>966</v>
@@ -14666,7 +14669,7 @@
         <v>1277</v>
       </c>
       <c r="X129" t="s">
-        <v>1393</v>
+        <v>1387</v>
       </c>
       <c r="AA129" t="s">
         <v>966</v>
@@ -14885,7 +14888,7 @@
         <v>1278</v>
       </c>
       <c r="X132" t="s">
-        <v>1394</v>
+        <v>1388</v>
       </c>
       <c r="AA132" t="s">
         <v>966</v>
@@ -16295,7 +16298,7 @@
         <v>1279</v>
       </c>
       <c r="X168" t="s">
-        <v>1395</v>
+        <v>1389</v>
       </c>
       <c r="AA168" t="s">
         <v>966</v>
@@ -16437,7 +16440,7 @@
         <v>1280</v>
       </c>
       <c r="X170" t="s">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="AA170" t="s">
         <v>759</v>
@@ -16718,7 +16721,7 @@
         <v>1225</v>
       </c>
       <c r="X174" t="s">
-        <v>1397</v>
+        <v>1391</v>
       </c>
       <c r="AA174" t="s">
         <v>966</v>
@@ -16860,7 +16863,7 @@
         <v>1281</v>
       </c>
       <c r="X176" t="s">
-        <v>1398</v>
+        <v>1392</v>
       </c>
       <c r="AA176" t="s">
         <v>759</v>
@@ -16931,7 +16934,7 @@
         <v>1282</v>
       </c>
       <c r="X177" t="s">
-        <v>1399</v>
+        <v>1393</v>
       </c>
       <c r="AA177" t="s">
         <v>966</v>
@@ -17014,7 +17017,7 @@
         <v>1283</v>
       </c>
       <c r="X178" t="s">
-        <v>1400</v>
+        <v>1394</v>
       </c>
       <c r="AA178" t="s">
         <v>966</v>
@@ -17728,7 +17731,7 @@
         <v>1284</v>
       </c>
       <c r="X187" t="s">
-        <v>1401</v>
+        <v>1395</v>
       </c>
       <c r="AA187" t="s">
         <v>759</v>
@@ -17948,7 +17951,7 @@
         <v>1286</v>
       </c>
       <c r="X190" t="s">
-        <v>1402</v>
+        <v>1396</v>
       </c>
       <c r="AA190" t="s">
         <v>966</v>
@@ -18022,7 +18025,7 @@
         <v>1287</v>
       </c>
       <c r="X191" t="s">
-        <v>1403</v>
+        <v>1397</v>
       </c>
       <c r="AA191" t="s">
         <v>966</v>
@@ -18250,7 +18253,7 @@
         <v>1288</v>
       </c>
       <c r="X194" t="s">
-        <v>1404</v>
+        <v>1398</v>
       </c>
       <c r="AA194" t="s">
         <v>966</v>
@@ -18330,7 +18333,7 @@
         <v>1289</v>
       </c>
       <c r="X195" t="s">
-        <v>1405</v>
+        <v>1399</v>
       </c>
       <c r="AA195" t="s">
         <v>966</v>
@@ -18632,7 +18635,7 @@
         <v>1291</v>
       </c>
       <c r="X199" t="s">
-        <v>1406</v>
+        <v>1400</v>
       </c>
       <c r="AA199" t="s">
         <v>966</v>
@@ -18718,7 +18721,7 @@
         <v>1292</v>
       </c>
       <c r="X200" t="s">
-        <v>1407</v>
+        <v>1401</v>
       </c>
       <c r="AA200" t="s">
         <v>966</v>
@@ -18875,7 +18878,7 @@
         <v>1293</v>
       </c>
       <c r="X202" t="s">
-        <v>1408</v>
+        <v>1402</v>
       </c>
       <c r="AA202" t="s">
         <v>966</v>
@@ -18958,7 +18961,7 @@
         <v>1294</v>
       </c>
       <c r="X203" t="s">
-        <v>1409</v>
+        <v>1403</v>
       </c>
       <c r="AA203" t="s">
         <v>966</v>
@@ -19171,7 +19174,7 @@
         <v>1295</v>
       </c>
       <c r="X206" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
       <c r="AA206" t="s">
         <v>966</v>
@@ -19390,7 +19393,7 @@
         <v>1297</v>
       </c>
       <c r="X209" t="s">
-        <v>1411</v>
+        <v>1405</v>
       </c>
       <c r="AA209" t="s">
         <v>966</v>
@@ -19541,7 +19544,7 @@
         <v>1298</v>
       </c>
       <c r="X211" t="s">
-        <v>1412</v>
+        <v>1406</v>
       </c>
       <c r="AA211" t="s">
         <v>966</v>
@@ -19615,7 +19618,7 @@
         <v>1299</v>
       </c>
       <c r="X212" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="AA212" t="s">
         <v>966</v>
@@ -19689,7 +19692,7 @@
         <v>1300</v>
       </c>
       <c r="X213" t="s">
-        <v>1414</v>
+        <v>1408</v>
       </c>
       <c r="AA213" t="s">
         <v>966</v>
@@ -19775,7 +19778,7 @@
         <v>1301</v>
       </c>
       <c r="X214" t="s">
-        <v>1415</v>
+        <v>1409</v>
       </c>
       <c r="AA214" t="s">
         <v>966</v>
@@ -20738,7 +20741,7 @@
         <v>1224</v>
       </c>
       <c r="X226" t="s">
-        <v>1416</v>
+        <v>1410</v>
       </c>
       <c r="AA226" t="s">
         <v>966</v>
@@ -20821,7 +20824,7 @@
         <v>1302</v>
       </c>
       <c r="X227" t="s">
-        <v>1417</v>
+        <v>1411</v>
       </c>
       <c r="AA227" t="s">
         <v>966</v>
@@ -20904,7 +20907,7 @@
         <v>1303</v>
       </c>
       <c r="X228" t="s">
-        <v>1418</v>
+        <v>1412</v>
       </c>
       <c r="AA228" t="s">
         <v>966</v>
@@ -21182,7 +21185,7 @@
         <v>1304</v>
       </c>
       <c r="X232" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="AA232" t="s">
         <v>966</v>
@@ -21265,7 +21268,7 @@
         <v>1305</v>
       </c>
       <c r="X233" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
       <c r="AA233" t="s">
         <v>966</v>
@@ -21348,7 +21351,7 @@
         <v>1306</v>
       </c>
       <c r="X234" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
       <c r="AA234" t="s">
         <v>966</v>
@@ -24450,7 +24453,7 @@
         <v>1307</v>
       </c>
       <c r="X273" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="AA273" t="s">
         <v>759</v>
@@ -24598,7 +24601,7 @@
         <v>1308</v>
       </c>
       <c r="X275" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="AA275" t="s">
         <v>966</v>
@@ -24758,7 +24761,7 @@
         <v>1310</v>
       </c>
       <c r="X277" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
       <c r="AA277" t="s">
         <v>966</v>
@@ -24838,7 +24841,7 @@
         <v>1311</v>
       </c>
       <c r="X278" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
       <c r="AA278" t="s">
         <v>966</v>
@@ -24918,7 +24921,7 @@
         <v>1312</v>
       </c>
       <c r="X279" t="s">
-        <v>1426</v>
+        <v>1454</v>
       </c>
       <c r="AA279" t="s">
         <v>966</v>
@@ -24998,7 +25001,7 @@
         <v>1313</v>
       </c>
       <c r="X280" t="s">
-        <v>1427</v>
+        <v>1420</v>
       </c>
       <c r="AA280" t="s">
         <v>966</v>
@@ -25421,7 +25424,7 @@
         <v>1315</v>
       </c>
       <c r="X286" t="s">
-        <v>1428</v>
+        <v>1421</v>
       </c>
       <c r="AA286" t="s">
         <v>966</v>
@@ -25863,7 +25866,7 @@
         <v>1316</v>
       </c>
       <c r="X292" t="s">
-        <v>1429</v>
+        <v>1422</v>
       </c>
       <c r="AA292" t="s">
         <v>966</v>
@@ -26150,7 +26153,7 @@
         <v>1317</v>
       </c>
       <c r="X296" t="s">
-        <v>1430</v>
+        <v>1423</v>
       </c>
       <c r="AA296" t="s">
         <v>759</v>
@@ -26173,19 +26176,19 @@
         <v>520</v>
       </c>
       <c r="C297" t="s">
-        <v>1457</v>
+        <v>1446</v>
       </c>
       <c r="D297">
         <v>0</v>
       </c>
       <c r="F297" t="s">
-        <v>1458</v>
+        <v>1447</v>
       </c>
       <c r="G297">
         <v>100</v>
       </c>
       <c r="H297" t="s">
-        <v>1458</v>
+        <v>1447</v>
       </c>
       <c r="I297" s="3" t="s">
         <v>521</v>
@@ -26295,7 +26298,7 @@
         <v>1318</v>
       </c>
       <c r="X298" t="s">
-        <v>1431</v>
+        <v>1424</v>
       </c>
       <c r="AA298" t="s">
         <v>966</v>
@@ -26449,7 +26452,7 @@
         <v>1319</v>
       </c>
       <c r="X300" t="s">
-        <v>1432</v>
+        <v>1425</v>
       </c>
       <c r="AA300" t="s">
         <v>966</v>
@@ -26526,7 +26529,7 @@
         <v>1320</v>
       </c>
       <c r="X301" t="s">
-        <v>1433</v>
+        <v>1426</v>
       </c>
       <c r="AA301" t="s">
         <v>966</v>
@@ -26677,7 +26680,7 @@
         <v>1321</v>
       </c>
       <c r="X303" t="s">
-        <v>1434</v>
+        <v>1427</v>
       </c>
       <c r="AA303" t="s">
         <v>966</v>
@@ -27130,7 +27133,7 @@
         <v>1322</v>
       </c>
       <c r="X309" t="s">
-        <v>1435</v>
+        <v>1428</v>
       </c>
       <c r="AA309" t="s">
         <v>966</v>
@@ -27210,7 +27213,7 @@
         <v>1323</v>
       </c>
       <c r="X310" t="s">
-        <v>1438</v>
+        <v>1431</v>
       </c>
       <c r="AA310" t="s">
         <v>759</v>
@@ -27355,7 +27358,7 @@
         <v>1324</v>
       </c>
       <c r="X312" t="s">
-        <v>1436</v>
+        <v>1429</v>
       </c>
       <c r="AA312" t="s">
         <v>966</v>
@@ -27426,7 +27429,7 @@
         <v>1263</v>
       </c>
       <c r="X313" t="s">
-        <v>1437</v>
+        <v>1430</v>
       </c>
       <c r="AA313" t="s">
         <v>966</v>
@@ -27500,7 +27503,7 @@
         <v>1325</v>
       </c>
       <c r="X314" t="s">
-        <v>1439</v>
+        <v>1432</v>
       </c>
       <c r="AA314" t="s">
         <v>966</v>
@@ -27583,7 +27586,7 @@
         <v>1326</v>
       </c>
       <c r="X315" t="s">
-        <v>1440</v>
+        <v>1455</v>
       </c>
       <c r="AA315" t="s">
         <v>966</v>
@@ -27870,7 +27873,7 @@
         <v>1328</v>
       </c>
       <c r="X319" t="s">
-        <v>1441</v>
+        <v>1433</v>
       </c>
       <c r="AA319" t="s">
         <v>966</v>
@@ -27944,7 +27947,7 @@
         <v>1254</v>
       </c>
       <c r="X320" t="s">
-        <v>1443</v>
+        <v>1434</v>
       </c>
       <c r="AA320" t="s">
         <v>759</v>
@@ -28024,7 +28027,7 @@
         <v>759</v>
       </c>
       <c r="X321" t="s">
-        <v>1444</v>
+        <v>1457</v>
       </c>
       <c r="AA321" t="s">
         <v>966</v>
@@ -28098,7 +28101,7 @@
         <v>1293</v>
       </c>
       <c r="X322" t="s">
-        <v>1408</v>
+        <v>1402</v>
       </c>
       <c r="AA322" t="s">
         <v>759</v>
@@ -28181,7 +28184,7 @@
         <v>1329</v>
       </c>
       <c r="X323" t="s">
-        <v>1445</v>
+        <v>1435</v>
       </c>
       <c r="AA323" t="s">
         <v>966</v>
@@ -28735,7 +28738,7 @@
         <v>1317</v>
       </c>
       <c r="X330" t="s">
-        <v>1446</v>
+        <v>1436</v>
       </c>
       <c r="AA330" t="s">
         <v>759</v>
@@ -28809,7 +28812,7 @@
         <v>1330</v>
       </c>
       <c r="X331" t="s">
-        <v>1359</v>
+        <v>1458</v>
       </c>
       <c r="AA331" t="s">
         <v>966</v>
@@ -28883,7 +28886,7 @@
         <v>1252</v>
       </c>
       <c r="X332" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="AA332" t="s">
         <v>966</v>
@@ -28957,7 +28960,7 @@
         <v>1331</v>
       </c>
       <c r="X333" t="s">
-        <v>1447</v>
+        <v>1437</v>
       </c>
       <c r="AA333" t="s">
         <v>966</v>
@@ -29028,7 +29031,7 @@
         <v>1332</v>
       </c>
       <c r="X334" t="s">
-        <v>1448</v>
+        <v>1438</v>
       </c>
       <c r="AA334" t="s">
         <v>759</v>
@@ -29111,7 +29114,7 @@
         <v>1333</v>
       </c>
       <c r="X335" t="s">
-        <v>1449</v>
+        <v>1439</v>
       </c>
       <c r="AA335" t="s">
         <v>966</v>
@@ -29905,7 +29908,7 @@
         <v>1334</v>
       </c>
       <c r="X345" t="s">
-        <v>1450</v>
+        <v>1440</v>
       </c>
       <c r="AA345" t="s">
         <v>966</v>
@@ -30127,7 +30130,7 @@
         <v>1335</v>
       </c>
       <c r="X348" t="s">
-        <v>1442</v>
+        <v>1456</v>
       </c>
       <c r="AA348" t="s">
         <v>966</v>
@@ -32559,7 +32562,7 @@
         <v>1336</v>
       </c>
       <c r="X379" t="s">
-        <v>1451</v>
+        <v>1441</v>
       </c>
       <c r="AA379" t="s">
         <v>966</v>
@@ -32630,7 +32633,7 @@
         <v>1238</v>
       </c>
       <c r="X380" t="s">
-        <v>1452</v>
+        <v>1442</v>
       </c>
       <c r="AE380" t="s">
         <v>708</v>
@@ -32775,7 +32778,7 @@
         <v>1337</v>
       </c>
       <c r="X382" t="s">
-        <v>1453</v>
+        <v>1443</v>
       </c>
       <c r="AA382" t="s">
         <v>966</v>
@@ -32911,7 +32914,7 @@
         <v>1338</v>
       </c>
       <c r="X384" t="s">
-        <v>1454</v>
+        <v>1459</v>
       </c>
       <c r="AA384" t="s">
         <v>966</v>
@@ -32994,7 +32997,7 @@
         <v>1339</v>
       </c>
       <c r="X385" t="s">
-        <v>1455</v>
+        <v>1444</v>
       </c>
       <c r="AA385" t="s">
         <v>966</v>
@@ -33880,7 +33883,7 @@
         <v>1340</v>
       </c>
       <c r="X396" t="s">
-        <v>1456</v>
+        <v>1445</v>
       </c>
       <c r="AA396" t="s">
         <v>966</v>

</xml_diff>

<commit_message>
Update TB data source to WHO 2024
</commit_message>
<xml_diff>
--- a/SourceData/globals/GBModData.xlsx
+++ b/SourceData/globals/GBModData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE038212-1307-4FC9-A169-F93BE3A0F37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EFF849-B027-44EA-A199-F4E84A84B4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4495,7 +4495,7 @@
     <t>Sample country_5733.upd</t>
   </si>
   <si>
-    <t>WHO 2023</t>
+    <t>WHO 2024</t>
   </si>
 </sst>
 </file>
@@ -4891,10 +4891,10 @@
   <dimension ref="A1:AJ416"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C233" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K365" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W29" sqref="W29"/>
+      <selection pane="bottomRight" activeCell="AB406" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39658,12 +39658,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -39869,15 +39866,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639808B5-4725-4AE9-9DF1-1833AC18DC8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39901,17 +39909,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639808B5-4725-4AE9-9DF1-1833AC18DC8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert TB source back to WHO 2023
</commit_message>
<xml_diff>
--- a/SourceData/globals/GBModData.xlsx
+++ b/SourceData/globals/GBModData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EFF849-B027-44EA-A199-F4E84A84B4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7629631F-1913-4D2D-AD6A-F353F0321AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4495,7 +4495,7 @@
     <t>Sample country_5733.upd</t>
   </si>
   <si>
-    <t>WHO 2024</t>
+    <t>WHO 2023</t>
   </si>
 </sst>
 </file>
@@ -4891,10 +4891,10 @@
   <dimension ref="A1:AJ416"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K365" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J296" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AB406" sqref="AB1:AB1048576"/>
+      <selection pane="bottomRight" activeCell="W315" sqref="W315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39658,9 +39658,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -39866,26 +39869,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639808B5-4725-4AE9-9DF1-1833AC18DC8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39909,9 +39901,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E04ADD-AF0C-45F3-A990-50A9A3A5EFA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639808B5-4725-4AE9-9DF1-1833AC18DC8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2c9bee02-199a-488a-b277-ba7f212fbf06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>